<commit_message>
Added Bank class to analyzer script
Added Bank class and initialized all items from the bank_statment.xlsx as objects of the class
</commit_message>
<xml_diff>
--- a/excel_python_oop_1/bank_statement.xlsx
+++ b/excel_python_oop_1/bank_statement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\GitHub\coding-for-fun-python\excel_python_oop_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2754CD6-3963-4D92-9044-59F7676AD53F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ADFDCE-E477-4882-9740-48EC18C166B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C736D445-5388-4816-BB21-D7A2F393BB2E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Some description D</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>BankA</t>
   </si>
 </sst>
 </file>
@@ -452,142 +458,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D43753B7-89EA-4903-A8C7-A8E1C608E051}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
         <v>44329</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>30</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1">
         <v>44330</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>2300</v>
       </c>
-      <c r="F3">
-        <f>F2-D3</f>
+      <c r="G3">
+        <f>G2-E3</f>
         <v>7700</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1">
         <v>44331</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>4500</v>
       </c>
-      <c r="F4">
-        <f t="shared" ref="F4:F5" si="0">F3-D4</f>
+      <c r="G4">
+        <f t="shared" ref="G4:G5" si="0">G3-E4</f>
         <v>3200</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
         <v>44332</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>25</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>3175</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
         <v>44333</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>8000</v>
       </c>
-      <c r="F6">
-        <f>F5+E6</f>
+      <c r="G6">
+        <f>G5+F6</f>
         <v>11175</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
         <v>44334</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>35</v>
       </c>
-      <c r="F7">
-        <f>F6-D7</f>
+      <c r="G7">
+        <f>G6-E7</f>
         <v>11140</v>
       </c>
     </row>

</xml_diff>